<commit_message>
adding the sckitlearn, openxl, install again the libraries
</commit_message>
<xml_diff>
--- a/1automatization-excel-word/files/1Distrito_poblacion.xlsx
+++ b/1automatization-excel-word/files/1Distrito_poblacion.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="figuras" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="other sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="other sheet1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,14 +453,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Huila</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="n">
-        <v>5</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Top 5</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>31.41592653589793</v>
@@ -565,4 +571,54 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Huila</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Top 5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>